<commit_message>
adding retry analyzer and headless options
</commit_message>
<xml_diff>
--- a/OrangeHRMProject/src/test/resources/testdata/Test_data.xlsx
+++ b/OrangeHRMProject/src/test/resources/testdata/Test_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="4476" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="4476"/>
   </bookViews>
   <sheets>
     <sheet name="validLoginTest" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -45,12 +45,6 @@
   </si>
   <si>
     <t>Vani Bhat</t>
-  </si>
-  <si>
-    <t>ashwin hebbar</t>
-  </si>
-  <si>
-    <t>sasha de della</t>
   </si>
 </sst>
 </file>
@@ -370,8 +364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,10 +424,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,22 +452,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
testing auto jenkins trigger
</commit_message>
<xml_diff>
--- a/OrangeHRMProject/src/test/resources/testdata/Test_data.xlsx
+++ b/OrangeHRMProject/src/test/resources/testdata/Test_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="4476"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="4476" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="validLoginTest" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Vani Bhat</t>
+  </si>
+  <si>
+    <t>ashwin hebbar</t>
   </si>
 </sst>
 </file>
@@ -364,7 +367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -424,10 +427,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,6 +455,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>